<commit_message>
Adición de analisis de diversidad de Ictio
</commit_message>
<xml_diff>
--- a/03_An_Expl_DatosBiologicos/Biologicos/DatosP_Ictioplancton/ICTIO_BOCASSanquianga.xlsx
+++ b/03_An_Expl_DatosBiologicos/Biologicos/DatosP_Ictioplancton/ICTIO_BOCASSanquianga.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2021\03_An_Expl_DatosBiologicos\Biologicos\DatosP_Ictioplancton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Expedición Pacífico\Ictioplancton_ExPacifico2021\03_An_Expl_DatosBiologicos\Biologicos\DatosP_Ictioplancton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A92884-B72F-4AF8-8A50-6903D13DAA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F8667E-749A-419C-A62A-BA8D356EB95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B1350CD-8E74-460B-8E60-1949550703E2}"/>
+    <workbookView xWindow="7680" yWindow="3120" windowWidth="28800" windowHeight="11385" activeTab="2" xr2:uid="{2B1350CD-8E74-460B-8E60-1949550703E2}"/>
   </bookViews>
   <sheets>
     <sheet name="MAREA BAJA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="16" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -448,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -466,7 +466,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1991,7 +1990,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{34D3CBE0-86DE-4E9A-AB9A-FC67507C9338}" name="TablaDinámica4" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{34D3CBE0-86DE-4E9A-AB9A-FC67507C9338}" name="TablaDinámica4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="U1:AM35" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField axis="axisRow" showAll="0">
@@ -2557,7 +2556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4458A694-22B0-454D-A63A-196C7937A37C}">
   <dimension ref="A1:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
@@ -4127,7 +4126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EE97D5-5EEB-4459-8D8C-259C2C9B6EBF}">
   <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView topLeftCell="AK13" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="V3" sqref="V3:AM3"/>
     </sheetView>
   </sheetViews>
@@ -4273,26 +4272,9 @@
       <c r="U2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11">
-        <v>2</v>
-      </c>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
+      <c r="W2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -4313,30 +4295,15 @@
       <c r="U3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11">
-        <v>2</v>
-      </c>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="11">
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3">
         <v>4</v>
       </c>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
-      <c r="AI3" s="11"/>
-      <c r="AJ3" s="11"/>
-      <c r="AK3" s="11"/>
-      <c r="AL3" s="11"/>
-      <c r="AM3" s="11"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -4351,28 +4318,12 @@
       <c r="U4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11">
+      <c r="Z4">
         <v>10</v>
       </c>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="11">
+      <c r="AI4">
         <v>10</v>
       </c>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="11"/>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="11"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -4387,30 +4338,15 @@
       <c r="U5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11">
+      <c r="AB5">
         <v>4</v>
       </c>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11">
-        <v>2</v>
-      </c>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11">
+      <c r="AD5">
+        <v>2</v>
+      </c>
+      <c r="AK5">
         <v>4</v>
       </c>
-      <c r="AL5" s="11"/>
-      <c r="AM5" s="11"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -4428,56 +4364,55 @@
       <c r="U6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="V6" s="11">
+      <c r="V6">
         <v>10</v>
       </c>
-      <c r="W6" s="11">
-        <v>2</v>
-      </c>
-      <c r="X6" s="11">
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
         <v>8</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Y6">
         <v>36</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6">
         <v>104</v>
       </c>
-      <c r="AA6" s="11">
+      <c r="AA6">
         <v>310</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6">
         <v>132</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6">
         <v>312</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AD6">
         <v>48</v>
       </c>
-      <c r="AE6" s="11">
+      <c r="AE6">
         <v>58</v>
       </c>
-      <c r="AF6" s="11">
+      <c r="AF6">
         <v>36</v>
       </c>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11">
+      <c r="AH6">
         <v>30</v>
       </c>
-      <c r="AI6" s="11">
+      <c r="AI6">
         <v>104</v>
       </c>
-      <c r="AJ6" s="11">
+      <c r="AJ6">
         <v>44</v>
       </c>
-      <c r="AK6" s="11">
+      <c r="AK6">
         <v>132</v>
       </c>
-      <c r="AL6" s="11">
+      <c r="AL6">
         <v>64</v>
       </c>
-      <c r="AM6" s="11">
+      <c r="AM6">
         <v>30</v>
       </c>
     </row>
@@ -4539,28 +4474,12 @@
       <c r="U7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11">
-        <v>2</v>
-      </c>
-      <c r="AF7" s="11">
-        <v>2</v>
-      </c>
-      <c r="AG7" s="11"/>
-      <c r="AH7" s="11"/>
-      <c r="AI7" s="11"/>
-      <c r="AJ7" s="11"/>
-      <c r="AK7" s="11"/>
-      <c r="AL7" s="11"/>
-      <c r="AM7" s="11"/>
+      <c r="AE7">
+        <v>2</v>
+      </c>
+      <c r="AF7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -4575,30 +4494,15 @@
       <c r="U8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11">
+      <c r="AA8">
         <v>10</v>
       </c>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11">
-        <v>2</v>
-      </c>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11">
+      <c r="AD8">
+        <v>2</v>
+      </c>
+      <c r="AJ8">
         <v>10</v>
       </c>
-      <c r="AK8" s="11"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -4622,28 +4526,12 @@
       <c r="U9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11">
-        <v>2</v>
-      </c>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11">
-        <v>2</v>
-      </c>
-      <c r="AG9" s="11"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
-      <c r="AJ9" s="11"/>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="11"/>
+      <c r="AC9">
+        <v>2</v>
+      </c>
+      <c r="AF9">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -4664,34 +4552,21 @@
       <c r="U10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11">
-        <v>2</v>
-      </c>
-      <c r="AA10" s="11">
-        <v>2</v>
-      </c>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11">
+      <c r="Z10">
+        <v>2</v>
+      </c>
+      <c r="AA10">
+        <v>2</v>
+      </c>
+      <c r="AC10">
         <v>4</v>
       </c>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="11"/>
-      <c r="AI10" s="11">
-        <v>2</v>
-      </c>
-      <c r="AJ10" s="11">
-        <v>2</v>
-      </c>
-      <c r="AK10" s="11"/>
-      <c r="AL10" s="11"/>
-      <c r="AM10" s="11"/>
+      <c r="AI10">
+        <v>2</v>
+      </c>
+      <c r="AJ10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -4721,38 +4596,27 @@
       <c r="U11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="V11" s="11">
+      <c r="V11">
         <v>224</v>
       </c>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11">
+      <c r="Z11">
         <v>4</v>
       </c>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11">
+      <c r="AB11">
         <v>52</v>
       </c>
-      <c r="AC11" s="11">
+      <c r="AC11">
         <v>8</v>
       </c>
-      <c r="AD11" s="11">
+      <c r="AD11">
         <v>4</v>
       </c>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11">
+      <c r="AG11">
         <v>26</v>
       </c>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="11">
+      <c r="AK11">
         <v>52</v>
       </c>
-      <c r="AL11" s="11"/>
-      <c r="AM11" s="11"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -4764,32 +4628,18 @@
       <c r="U12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="V12" s="11">
-        <v>2</v>
-      </c>
-      <c r="W12" s="11">
+      <c r="V12">
+        <v>2</v>
+      </c>
+      <c r="W12">
         <v>6</v>
       </c>
-      <c r="X12" s="11">
-        <v>2</v>
-      </c>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11">
-        <v>2</v>
-      </c>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="11"/>
-      <c r="AK12" s="11"/>
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="11"/>
+      <c r="X12">
+        <v>2</v>
+      </c>
+      <c r="AE12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -4816,26 +4666,9 @@
       <c r="U13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="V13" s="11">
-        <v>2</v>
-      </c>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
+      <c r="V13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -4847,36 +4680,24 @@
       <c r="U14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11">
-        <v>2</v>
-      </c>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11">
+      <c r="Y14">
+        <v>2</v>
+      </c>
+      <c r="AB14">
         <v>26</v>
       </c>
-      <c r="AC14" s="11">
+      <c r="AC14">
         <v>12</v>
       </c>
-      <c r="AD14" s="11">
+      <c r="AD14">
         <v>32</v>
       </c>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11">
-        <v>2</v>
-      </c>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11">
+      <c r="AH14">
+        <v>2</v>
+      </c>
+      <c r="AK14">
         <v>26</v>
       </c>
-      <c r="AL14" s="11"/>
-      <c r="AM14" s="11"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -4894,26 +4715,9 @@
       <c r="U15" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11">
-        <v>2</v>
-      </c>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="11"/>
-      <c r="AK15" s="11"/>
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="11"/>
+      <c r="AF15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -4925,26 +4729,9 @@
       <c r="U16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11">
-        <v>2</v>
-      </c>
-      <c r="AH16" s="11"/>
-      <c r="AI16" s="11"/>
-      <c r="AJ16" s="11"/>
-      <c r="AK16" s="11"/>
-      <c r="AL16" s="11"/>
-      <c r="AM16" s="11"/>
+      <c r="AG16">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -4962,26 +4749,9 @@
       <c r="U17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="V17" s="11">
-        <v>2</v>
-      </c>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
-      <c r="AI17" s="11"/>
-      <c r="AJ17" s="11"/>
-      <c r="AK17" s="11"/>
-      <c r="AL17" s="11"/>
-      <c r="AM17" s="11"/>
+      <c r="V17">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -4996,30 +4766,15 @@
       <c r="U18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="V18" s="11">
+      <c r="V18">
         <v>4</v>
       </c>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11">
+      <c r="AA18">
         <v>4</v>
       </c>
-      <c r="AB18" s="11">
-        <v>2</v>
-      </c>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="11"/>
-      <c r="AI18" s="11"/>
-      <c r="AJ18" s="11"/>
-      <c r="AK18" s="11"/>
-      <c r="AL18" s="11"/>
-      <c r="AM18" s="11"/>
+      <c r="AB18">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -5037,24 +4792,6 @@
       <c r="U19" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
-      <c r="AD19" s="11"/>
-      <c r="AE19" s="11"/>
-      <c r="AF19" s="11"/>
-      <c r="AG19" s="11"/>
-      <c r="AH19" s="11"/>
-      <c r="AI19" s="11"/>
-      <c r="AJ19" s="11"/>
-      <c r="AK19" s="11"/>
-      <c r="AL19" s="11"/>
-      <c r="AM19" s="11"/>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -5072,42 +4809,33 @@
       <c r="U20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="V20" s="11">
-        <v>2</v>
-      </c>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11">
+      <c r="V20">
+        <v>2</v>
+      </c>
+      <c r="X20">
         <v>28</v>
       </c>
-      <c r="Y20" s="11">
+      <c r="Y20">
         <v>4</v>
       </c>
-      <c r="Z20" s="11">
+      <c r="Z20">
         <v>14</v>
       </c>
-      <c r="AA20" s="11">
+      <c r="AA20">
         <v>20</v>
       </c>
-      <c r="AB20" s="11">
+      <c r="AB20">
         <v>44</v>
       </c>
-      <c r="AC20" s="11">
+      <c r="AC20">
         <v>16</v>
       </c>
-      <c r="AD20" s="11"/>
-      <c r="AE20" s="11">
+      <c r="AE20">
         <v>16</v>
       </c>
-      <c r="AF20" s="11"/>
-      <c r="AG20" s="11"/>
-      <c r="AH20" s="11"/>
-      <c r="AI20" s="11"/>
-      <c r="AJ20" s="11"/>
-      <c r="AK20" s="11"/>
-      <c r="AL20" s="11">
+      <c r="AL20">
         <v>8</v>
       </c>
-      <c r="AM20" s="11"/>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -5125,30 +4853,15 @@
       <c r="U21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="11"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="11">
+      <c r="AC21">
         <v>12</v>
       </c>
-      <c r="AD21" s="11">
-        <v>2</v>
-      </c>
-      <c r="AE21" s="11">
-        <v>2</v>
-      </c>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="11"/>
-      <c r="AH21" s="11"/>
-      <c r="AI21" s="11"/>
-      <c r="AJ21" s="11"/>
-      <c r="AK21" s="11"/>
-      <c r="AL21" s="11"/>
-      <c r="AM21" s="11"/>
+      <c r="AD21">
+        <v>2</v>
+      </c>
+      <c r="AE21">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -5181,28 +4894,12 @@
       <c r="U22" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11">
-        <v>2</v>
-      </c>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11">
-        <v>2</v>
-      </c>
-      <c r="AI22" s="11"/>
-      <c r="AJ22" s="11"/>
-      <c r="AK22" s="11"/>
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="11"/>
+      <c r="Y22">
+        <v>2</v>
+      </c>
+      <c r="AH22">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -5223,28 +4920,13 @@
       <c r="U23" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11">
-        <v>2</v>
-      </c>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="11"/>
-      <c r="AC23" s="11"/>
-      <c r="AD23" s="11"/>
-      <c r="AE23" s="11"/>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="11"/>
-      <c r="AH23" s="11">
-        <v>2</v>
-      </c>
-      <c r="AI23" s="11"/>
-      <c r="AJ23" s="11"/>
-      <c r="AK23" s="11"/>
-      <c r="AL23" s="11"/>
-      <c r="AM23" s="11">
+      <c r="Y23">
+        <v>2</v>
+      </c>
+      <c r="AH23">
+        <v>2</v>
+      </c>
+      <c r="AM23">
         <v>4</v>
       </c>
     </row>
@@ -5255,28 +4937,13 @@
       <c r="U24" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11">
-        <v>2</v>
-      </c>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-      <c r="AE24" s="11"/>
-      <c r="AF24" s="11"/>
-      <c r="AG24" s="11"/>
-      <c r="AH24" s="11"/>
-      <c r="AI24" s="11"/>
-      <c r="AJ24" s="11">
-        <v>2</v>
-      </c>
-      <c r="AK24" s="11"/>
-      <c r="AL24" s="11"/>
-      <c r="AM24" s="11">
+      <c r="AA24">
+        <v>2</v>
+      </c>
+      <c r="AJ24">
+        <v>2</v>
+      </c>
+      <c r="AM24">
         <v>12</v>
       </c>
     </row>
@@ -5296,40 +4963,30 @@
       <c r="U25" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11">
-        <v>2</v>
-      </c>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="11">
+      <c r="X25">
+        <v>2</v>
+      </c>
+      <c r="AA25">
         <v>54</v>
       </c>
-      <c r="AB25" s="11">
+      <c r="AB25">
         <v>24</v>
       </c>
-      <c r="AC25" s="11">
+      <c r="AC25">
         <v>4</v>
       </c>
-      <c r="AD25" s="11"/>
-      <c r="AE25" s="11">
+      <c r="AE25">
         <v>4</v>
       </c>
-      <c r="AF25" s="11"/>
-      <c r="AG25" s="11">
+      <c r="AG25">
         <v>8</v>
       </c>
-      <c r="AH25" s="11"/>
-      <c r="AI25" s="11"/>
-      <c r="AJ25" s="11">
+      <c r="AJ25">
         <v>54</v>
       </c>
-      <c r="AK25" s="11">
+      <c r="AK25">
         <v>24</v>
       </c>
-      <c r="AL25" s="11"/>
-      <c r="AM25" s="11"/>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -5344,48 +5001,43 @@
       <c r="U26" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="V26" s="11">
+      <c r="V26">
         <v>4</v>
       </c>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11">
-        <v>2</v>
-      </c>
-      <c r="Y26" s="11">
+      <c r="X26">
+        <v>2</v>
+      </c>
+      <c r="Y26">
         <v>6</v>
       </c>
-      <c r="Z26" s="11">
+      <c r="Z26">
         <v>8</v>
       </c>
-      <c r="AA26" s="11">
+      <c r="AA26">
         <v>4</v>
       </c>
-      <c r="AB26" s="11">
+      <c r="AB26">
         <v>14</v>
       </c>
-      <c r="AC26" s="11">
+      <c r="AC26">
         <v>8</v>
       </c>
-      <c r="AD26" s="11"/>
-      <c r="AE26" s="11">
-        <v>2</v>
-      </c>
-      <c r="AF26" s="11"/>
-      <c r="AG26" s="11">
+      <c r="AE26">
+        <v>2</v>
+      </c>
+      <c r="AG26">
         <v>4</v>
       </c>
-      <c r="AH26" s="11"/>
-      <c r="AI26" s="11">
+      <c r="AI26">
         <v>24</v>
       </c>
-      <c r="AJ26" s="11">
-        <v>2</v>
-      </c>
-      <c r="AK26" s="11"/>
-      <c r="AL26" s="11">
+      <c r="AJ26">
+        <v>2</v>
+      </c>
+      <c r="AL26">
         <v>4</v>
       </c>
-      <c r="AM26" s="11">
+      <c r="AM26">
         <v>2</v>
       </c>
     </row>
@@ -5399,24 +5051,6 @@
       <c r="U27" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="11"/>
-      <c r="AF27" s="11"/>
-      <c r="AG27" s="11"/>
-      <c r="AH27" s="11"/>
-      <c r="AI27" s="11"/>
-      <c r="AJ27" s="11"/>
-      <c r="AK27" s="11"/>
-      <c r="AL27" s="11"/>
-      <c r="AM27" s="11"/>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -5464,28 +5098,12 @@
       <c r="U28" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
-      <c r="AD28" s="11">
-        <v>2</v>
-      </c>
-      <c r="AE28" s="11">
-        <v>2</v>
-      </c>
-      <c r="AF28" s="11"/>
-      <c r="AG28" s="11"/>
-      <c r="AH28" s="11"/>
-      <c r="AI28" s="11"/>
-      <c r="AJ28" s="11"/>
-      <c r="AK28" s="11"/>
-      <c r="AL28" s="11"/>
-      <c r="AM28" s="11"/>
+      <c r="AD28">
+        <v>2</v>
+      </c>
+      <c r="AE28">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -5494,32 +5112,18 @@
       <c r="U29" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11">
+      <c r="Y29">
         <v>6</v>
       </c>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="11"/>
-      <c r="AB29" s="11"/>
-      <c r="AC29" s="11"/>
-      <c r="AD29" s="11"/>
-      <c r="AE29" s="11"/>
-      <c r="AF29" s="11"/>
-      <c r="AG29" s="11"/>
-      <c r="AH29" s="11">
+      <c r="AH29">
         <v>6</v>
       </c>
-      <c r="AI29" s="11"/>
-      <c r="AJ29" s="11">
+      <c r="AJ29">
         <v>8</v>
       </c>
-      <c r="AK29" s="11"/>
-      <c r="AL29" s="11">
+      <c r="AL29">
         <v>10</v>
       </c>
-      <c r="AM29" s="11"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -5534,26 +5138,9 @@
       <c r="U30" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11">
+      <c r="Z30">
         <v>4</v>
       </c>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="11"/>
-      <c r="AC30" s="11"/>
-      <c r="AD30" s="11"/>
-      <c r="AE30" s="11"/>
-      <c r="AF30" s="11"/>
-      <c r="AG30" s="11"/>
-      <c r="AH30" s="11"/>
-      <c r="AI30" s="11"/>
-      <c r="AJ30" s="11"/>
-      <c r="AK30" s="11"/>
-      <c r="AL30" s="11"/>
-      <c r="AM30" s="11"/>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -5565,26 +5152,9 @@
       <c r="U31" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
-      <c r="AA31" s="11"/>
-      <c r="AB31" s="11"/>
-      <c r="AC31" s="11"/>
-      <c r="AD31" s="11">
-        <v>2</v>
-      </c>
-      <c r="AE31" s="11"/>
-      <c r="AF31" s="11"/>
-      <c r="AG31" s="11"/>
-      <c r="AH31" s="11"/>
-      <c r="AI31" s="11"/>
-      <c r="AJ31" s="11"/>
-      <c r="AK31" s="11"/>
-      <c r="AL31" s="11"/>
-      <c r="AM31" s="11"/>
+      <c r="AD31">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -5596,32 +5166,18 @@
       <c r="U32" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11">
-        <v>2</v>
-      </c>
-      <c r="AA32" s="11">
+      <c r="Z32">
+        <v>2</v>
+      </c>
+      <c r="AA32">
         <v>10</v>
       </c>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11">
-        <v>2</v>
-      </c>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="11">
+      <c r="AC32">
+        <v>2</v>
+      </c>
+      <c r="AE32">
         <v>4</v>
       </c>
-      <c r="AF32" s="11"/>
-      <c r="AG32" s="11"/>
-      <c r="AH32" s="11"/>
-      <c r="AI32" s="11"/>
-      <c r="AJ32" s="11"/>
-      <c r="AK32" s="11"/>
-      <c r="AL32" s="11"/>
-      <c r="AM32" s="11"/>
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -5633,30 +5189,15 @@
       <c r="U33" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11">
+      <c r="Z33">
         <v>12</v>
       </c>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
-      <c r="AE33" s="11"/>
-      <c r="AF33" s="11"/>
-      <c r="AG33" s="11"/>
-      <c r="AH33" s="11"/>
-      <c r="AI33" s="11">
+      <c r="AI33">
         <v>12</v>
       </c>
-      <c r="AJ33" s="11"/>
-      <c r="AK33" s="11"/>
-      <c r="AL33" s="11">
-        <v>2</v>
-      </c>
-      <c r="AM33" s="11"/>
+      <c r="AL33">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -5692,28 +5233,12 @@
       <c r="U34" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="V34" s="11"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="11"/>
-      <c r="Y34" s="11"/>
-      <c r="Z34" s="11"/>
-      <c r="AA34" s="11"/>
-      <c r="AB34" s="11"/>
-      <c r="AC34" s="11"/>
-      <c r="AD34" s="11"/>
-      <c r="AE34" s="11">
-        <v>2</v>
-      </c>
-      <c r="AF34" s="11">
+      <c r="AE34">
+        <v>2</v>
+      </c>
+      <c r="AF34">
         <v>4</v>
       </c>
-      <c r="AG34" s="11"/>
-      <c r="AH34" s="11"/>
-      <c r="AI34" s="11"/>
-      <c r="AJ34" s="11"/>
-      <c r="AK34" s="11"/>
-      <c r="AL34" s="11"/>
-      <c r="AM34" s="11"/>
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
@@ -5731,58 +5256,58 @@
       <c r="U35" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="V35" s="11">
+      <c r="V35">
         <v>250</v>
       </c>
-      <c r="W35" s="11">
+      <c r="W35">
         <v>10</v>
       </c>
-      <c r="X35" s="11">
+      <c r="X35">
         <v>44</v>
       </c>
-      <c r="Y35" s="11">
+      <c r="Y35">
         <v>58</v>
       </c>
-      <c r="Z35" s="11">
+      <c r="Z35">
         <v>160</v>
       </c>
-      <c r="AA35" s="11">
+      <c r="AA35">
         <v>416</v>
       </c>
-      <c r="AB35" s="11">
+      <c r="AB35">
         <v>298</v>
       </c>
-      <c r="AC35" s="11">
+      <c r="AC35">
         <v>382</v>
       </c>
-      <c r="AD35" s="11">
+      <c r="AD35">
         <v>98</v>
       </c>
-      <c r="AE35" s="11">
+      <c r="AE35">
         <v>94</v>
       </c>
-      <c r="AF35" s="11">
+      <c r="AF35">
         <v>46</v>
       </c>
-      <c r="AG35" s="11">
+      <c r="AG35">
         <v>40</v>
       </c>
-      <c r="AH35" s="11">
+      <c r="AH35">
         <v>42</v>
       </c>
-      <c r="AI35" s="11">
+      <c r="AI35">
         <v>152</v>
       </c>
-      <c r="AJ35" s="11">
+      <c r="AJ35">
         <v>122</v>
       </c>
-      <c r="AK35" s="11">
+      <c r="AK35">
         <v>238</v>
       </c>
-      <c r="AL35" s="11">
+      <c r="AL35">
         <v>88</v>
       </c>
-      <c r="AM35" s="11">
+      <c r="AM35">
         <v>48</v>
       </c>
     </row>
@@ -6306,8 +5831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE26E8CF-AE4D-4228-BB48-769272256159}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7104,10 +6629,10 @@
       <c r="B1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -7116,13 +6641,13 @@
       <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -9156,23 +8681,23 @@
         <v>2</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="11" t="s">
         <v>31</v>
       </c>
       <c r="J21" s="3" t="s">

</xml_diff>

<commit_message>
Adición de modelos espaciales
</commit_message>
<xml_diff>
--- a/03_An_Expl_DatosBiologicos/Biologicos/DatosP_Ictioplancton/ICTIO_BOCASSanquianga.xlsx
+++ b/03_An_Expl_DatosBiologicos/Biologicos/DatosP_Ictioplancton/ICTIO_BOCASSanquianga.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Expedicion_Pacifico\2021\Ictioplancton\Analisis_Exp_Pac\Ictioplancton_ExPacifico2021\03_An_Expl_DatosBiologicos\Biologicos\DatosP_Ictioplancton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Expedición Pacífico\Ictioplancton_ExPacifico2021\03_An_Expl_DatosBiologicos\Biologicos\DatosP_Ictioplancton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5AB637-263C-4528-B91B-A122CE49010F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0A749B-988C-4573-9A4B-63B69B92E397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2B1350CD-8E74-460B-8E60-1949550703E2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="2" xr2:uid="{2B1350CD-8E74-460B-8E60-1949550703E2}"/>
   </bookViews>
   <sheets>
     <sheet name="MAREA BAJA" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja6" sheetId="8" r:id="rId2"/>
     <sheet name="MAREA ALTA" sheetId="2" r:id="rId3"/>
     <sheet name="Hoja5" sheetId="7" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="112">
   <si>
     <t>Familia</t>
   </si>
@@ -2557,7 +2558,7 @@
   <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+      <selection sqref="A1:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4126,8 +4127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EE97D5-5EEB-4459-8D8C-259C2C9B6EBF}">
   <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3:AM3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5832,7 +5833,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V28"/>
+      <selection activeCell="A2" sqref="A2:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6589,7 +6590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD661E61-F4FA-4EE0-9E10-3B416B26B829}">
   <dimension ref="A1:AJ39"/>
   <sheetViews>
-    <sheetView topLeftCell="Z13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22:AJ39"/>
     </sheetView>
   </sheetViews>
@@ -10375,4 +10376,192 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE76B816-4F67-49D6-B7A6-F425BB16D54F}">
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>